<commit_message>
Fixed weather reporter sequence
</commit_message>
<xml_diff>
--- a/SOFTENG_762_Group_10/data.xlsx
+++ b/SOFTENG_762_Group_10/data.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\UiPath\SE762_Group10\SOFTENG_762_Group_10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omad882\Documents\UiPath\SE762_Group10\SOFTENG_762_Group_10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0DA1B1-A438-49A6-B7D4-E3173DC87013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4895A4-D2A0-4B6D-BD13-408D39DEDAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>location</t>
   </si>
@@ -42,6 +41,12 @@
     <t>Kumeu</t>
   </si>
   <si>
+    <t>Eastern Rangitaiki</t>
+  </si>
+  <si>
+    <t>Methven</t>
+  </si>
+  <si>
     <t>date</t>
   </si>
   <si>
@@ -51,22 +56,10 @@
     <t>max_temp</t>
   </si>
   <si>
-    <t>Fri 6 Oct</t>
-  </si>
-  <si>
-    <t>18°</t>
-  </si>
-  <si>
-    <t>11°</t>
+    <t>email</t>
   </si>
   <si>
     <t>samft223@gmail.com</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>images</t>
   </si>
   <si>
     <t>SOFTENG762Group10@gmail.com</t>
@@ -118,17 +111,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -407,245 +399,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16 F16"/>
+      <selection activeCell="A7" sqref="A7 A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DF58D4-B58D-4CD2-B948-F83847571D0F}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E576FF-D14B-4CD8-B020-A7C02C29F920}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9 B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DF58D4-B58D-4CD2-B948-F83847571D0F}">
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P23" sqref="P23 P23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E576FF-D14B-4CD8-B020-A7C02C29F920}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A3" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{D24E6C12-ACA9-4D4E-958E-DC6374CBB7F9}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{9165C0B0-1AAD-4DE1-B33B-2CAFA16FADE2}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D6C62A-33DB-4CD3-97BA-1EEC8406D933}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed email, multiple warnings WIP
</commit_message>
<xml_diff>
--- a/SOFTENG_762_Group_10/data.xlsx
+++ b/SOFTENG_762_Group_10/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omad882\Documents\UiPath\SE762_Group10\SOFTENG_762_Group_10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4895A4-D2A0-4B6D-BD13-408D39DEDAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D0D1B8-CD16-4F7D-A3E7-53E7556458B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>location</t>
   </si>
@@ -56,13 +56,31 @@
     <t>max_temp</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>samft223@gmail.com</t>
+    <t>Mon 9 Oct</t>
+  </si>
+  <si>
+    <t>16°</t>
+  </si>
+  <si>
+    <t>12°</t>
+  </si>
+  <si>
+    <t>17°</t>
+  </si>
+  <si>
+    <t>11°</t>
+  </si>
+  <si>
+    <t>14°</t>
+  </si>
+  <si>
+    <t>4°</t>
   </si>
   <si>
     <t>SOFTENG762Group10@gmail.com</t>
+  </si>
+  <si>
+    <t>emails</t>
   </si>
 </sst>
 </file>
@@ -445,13 +463,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DF58D4-B58D-4CD2-B948-F83847571D0F}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -467,6 +488,76 @@
         <v>8</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -474,34 +565,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E576FF-D14B-4CD8-B020-A7C02C29F920}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9 B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
+      <c r="A1" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>